<commit_message>
Verified imported data for COA
</commit_message>
<xml_diff>
--- a/testdata/imports/COA/Chartofaccountsexcelformat.xlsx
+++ b/testdata/imports/COA/Chartofaccountsexcelformat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Auto2020\WebAuto\web-automation-java\testdata\imports\COA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWB-Import\web-automation-java\testdata\imports\COA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Account Code</t>
   </si>
@@ -41,16 +41,19 @@
     <t>Tax Code</t>
   </si>
   <si>
-    <t>BANK ACCOUNT</t>
-  </si>
-  <si>
     <t>Bank</t>
   </si>
   <si>
     <t>OP (0%)</t>
   </si>
   <si>
-    <t>BANK ACC</t>
+    <t>BA000020</t>
+  </si>
+  <si>
+    <t>TestBankAccountBA20</t>
+  </si>
+  <si>
+    <t>Test description</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -402,19 +405,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>